<commit_message>
Update Bug report excel
</commit_message>
<xml_diff>
--- a/Bug_report_CheckList.xlsx
+++ b/Bug_report_CheckList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EEEF05FF-8997-4462-BE8F-49C2CE1458CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2851E21E-63F3-4905-BC8A-3A15A15B7214}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" xr2:uid="{295F6403-4D3D-4112-9931-82F0F9397295}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="18900" windowHeight="11175" xr2:uid="{295F6403-4D3D-4112-9931-82F0F9397295}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -3215,16 +3215,16 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -3699,7 +3699,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>4974248</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>2842571</xdr:rowOff>
+      <xdr:rowOff>2842572</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4519,19 +4519,17 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="61.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="111.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="1"/>
-    <col min="7" max="7" width="94.140625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -4671,7 +4669,7 @@
       </c>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:5" ht="313.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="333" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -4735,7 +4733,7 @@
       <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="17" t="s">
         <v>33</v>
       </c>
       <c r="C14" s="14" t="s">
@@ -4750,7 +4748,7 @@
       <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="16"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="14" t="s">
         <v>5</v>
       </c>
@@ -4781,7 +4779,7 @@
       <c r="B17" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="15" t="s">
         <v>4</v>
       </c>
       <c r="D17" s="7" t="s">
@@ -4850,10 +4848,10 @@
       <c r="E21" s="9"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="16" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>